<commit_message>
feat: add registry URL handling and update progress display in FixIncome components
</commit_message>
<xml_diff>
--- a/assets/Plantilla-Operacion.xlsx
+++ b/assets/Plantilla-Operacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\proyectos-web\inversorhouse-web\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4E1764-FA91-4DB2-A12D-667ED5305365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60305D4F-6D01-477E-A743-5479C7D955EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A9FBD9E-D8FD-47FD-9CB6-C19224A81F71}"/>
   </bookViews>
@@ -32,6 +32,49 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Alejandro Javier Del Medico Bravo</author>
+  </authors>
+  <commentList>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{64D5761D-8B11-4450-86A3-5C2E6BF85D5B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Los </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DATOS OPERACIÓN</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> son aproximados, estimados en base a la mayoria de operaciones.
+Es reponsabilidad de gestor ajustar estos valores de forma precisa para la operación correspondiente.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
@@ -78,9 +121,6 @@
   </si>
   <si>
     <t>Presupuesto desocupación</t>
-  </si>
-  <si>
-    <t>Otros gatos</t>
   </si>
   <si>
     <t>Reforma</t>
@@ -212,6 +252,9 @@
   <si>
     <t>Gastos de gestión</t>
   </si>
+  <si>
+    <t>Otros gastos</t>
+  </si>
 </sst>
 </file>
 
@@ -220,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +410,19 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -856,6 +912,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1174,11 +1234,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F1F55E-C7E8-4300-85DF-4985FB3E3E58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F1F55E-C7E8-4300-85DF-4985FB3E3E58}">
   <dimension ref="A1:AD80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13.8"/>
@@ -1201,7 +1261,7 @@
     <row r="2" spans="1:30" ht="87.6" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
@@ -1279,10 +1339,10 @@
     <row r="5" spans="1:30" ht="15" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>12</v>
@@ -1355,7 +1415,7 @@
     <row r="7" spans="1:30" ht="15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>3</v>
@@ -1497,23 +1557,23 @@
     <row r="11" spans="1:30" ht="15" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1538,9 +1598,7 @@
     </row>
     <row r="12" spans="1:30" ht="19.95" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
+      <c r="B12" s="12"/>
       <c r="C12" s="14">
         <v>0.1</v>
       </c>
@@ -1549,18 +1607,18 @@
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <f>B12*0.08</f>
+        <f>(B12*0.08)*1.21</f>
         <v>0</v>
       </c>
       <c r="F12" s="17">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G12" s="12">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H12" s="18">
         <f>B12+D12+E12+F12+G12</f>
-        <v>0</v>
+        <v>10500</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1612,7 +1670,7 @@
     <row r="14" spans="1:30" ht="14.4">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1646,25 +1704,25 @@
     <row r="15" spans="1:30" ht="15" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="16" t="s">
         <v>18</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>19</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1692,26 +1750,26 @@
     <row r="16" spans="1:30" ht="19.95" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="C16" s="12">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D16" s="12">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E16" s="12">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="F16" s="12">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H16" s="18">
         <f>SUM(B16:G16)</f>
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1771,7 +1829,7 @@
     <row r="18" spans="1:30" ht="14.4">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1805,13 +1863,13 @@
     <row r="19" spans="1:30" ht="15" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="D19" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -1846,10 +1904,10 @@
         <v>0.05</v>
       </c>
       <c r="C20" s="22">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D20" s="23">
-        <v>10000</v>
+        <v>25000</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1913,7 +1971,7 @@
     <row r="22" spans="1:30">
       <c r="A22" s="1"/>
       <c r="B22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1948,13 +2006,13 @@
         <v>9</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1985,17 +2043,14 @@
     <row r="24" spans="1:30" ht="19.95" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="12">
-        <v>1</v>
-      </c>
-      <c r="D24" s="12">
-        <v>2</v>
-      </c>
-      <c r="E24" s="12">
-        <v>3</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="18">
+        <f>(E24+C24)/2</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2025,19 +2080,19 @@
     <row r="25" spans="1:30" ht="19.95" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="18">
         <f>C24*$B$20</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D25" s="18">
         <f>D24*$B$20</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="18">
         <f>E24*$B$20</f>
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -2068,19 +2123,19 @@
     <row r="26" spans="1:30" ht="19.95" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="18">
         <f>C25+$H$12+$H$16</f>
-        <v>0.05</v>
+        <v>22500</v>
       </c>
       <c r="D26" s="18">
         <f>D25+$H$12+$H$16</f>
-        <v>0.1</v>
+        <v>22500</v>
       </c>
       <c r="E26" s="18">
         <f>E25+$H$12+$H$16</f>
-        <v>0.15000000000000002</v>
+        <v>22500</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2111,19 +2166,19 @@
     <row r="27" spans="1:30" ht="19.95" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="18">
         <f>C24-C26</f>
-        <v>0.95</v>
+        <v>-22500</v>
       </c>
       <c r="D27" s="18">
         <f t="shared" ref="D27:E27" si="0">D24-D26</f>
-        <v>1.9</v>
+        <v>-22500</v>
       </c>
       <c r="E27" s="18">
         <f t="shared" si="0"/>
-        <v>2.85</v>
+        <v>-22500</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -2158,15 +2213,15 @@
       </c>
       <c r="C28" s="19">
         <f>C27/C26</f>
-        <v>18.999999999999996</v>
+        <v>-1</v>
       </c>
       <c r="D28" s="19">
         <f t="shared" ref="D28:E28" si="1">D27/D26</f>
-        <v>18.999999999999996</v>
+        <v>-1</v>
       </c>
       <c r="E28" s="19">
         <f t="shared" si="1"/>
-        <v>18.999999999999996</v>
+        <v>-1</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2197,19 +2252,19 @@
     <row r="29" spans="1:30" ht="19.95" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="25">
         <f>(C24-C26)*$C$20</f>
-        <v>0.19</v>
+        <v>-6750</v>
       </c>
       <c r="D29" s="25">
         <f>(D24-D26)*$C$20</f>
-        <v>0.38</v>
+        <v>-6750</v>
       </c>
       <c r="E29" s="25">
         <f>(E24-E26)*$C$20</f>
-        <v>0.57000000000000006</v>
+        <v>-6750</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2240,19 +2295,19 @@
     <row r="30" spans="1:30" ht="19.95" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="31">
         <f>$D$20/C26</f>
-        <v>200000</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="D30" s="31">
         <f>$D$20/D26</f>
-        <v>100000</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="E30" s="31">
         <f>$D$20/E26</f>
-        <v>66666.666666666657</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -2283,19 +2338,19 @@
     <row r="31" spans="1:30" ht="19.95" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="32">
         <f>(C27-C29)*C30</f>
-        <v>152000</v>
+        <v>-17500</v>
       </c>
       <c r="D31" s="32">
         <f t="shared" ref="D31:E31" si="2">(D27-D29)*D30</f>
-        <v>152000</v>
+        <v>-17500</v>
       </c>
       <c r="E31" s="32">
         <f t="shared" si="2"/>
-        <v>152000</v>
+        <v>-17500</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -2358,7 +2413,7 @@
     <row r="33" spans="1:30" s="28" customFormat="1" ht="70.05" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
@@ -3684,10 +3739,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: implement profit calculator and update opportunity views to use calculated rentability
</commit_message>
<xml_diff>
--- a/assets/Plantilla-Operacion.xlsx
+++ b/assets/Plantilla-Operacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\proyectos-web\inversorhouse-web\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60305D4F-6D01-477E-A743-5479C7D955EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666F9A53-C347-4B02-871B-E5A863DA5AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A9FBD9E-D8FD-47FD-9CB6-C19224A81F71}"/>
   </bookViews>
@@ -914,10 +914,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1607,18 +1603,19 @@
         <v>0</v>
       </c>
       <c r="E12" s="18">
-        <f>(B12*0.08)*1.21</f>
+        <f>(B12*0.06)*1.21</f>
         <v>0</v>
       </c>
       <c r="F12" s="17">
-        <v>10000</v>
+        <f>IF(B8="Sí",10000,0)</f>
+        <v>0</v>
       </c>
       <c r="G12" s="12">
         <v>500</v>
       </c>
       <c r="H12" s="18">
         <f>B12+D12+E12+F12+G12</f>
-        <v>10500</v>
+        <v>500</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1901,7 +1898,7 @@
     <row r="20" spans="1:30" ht="19.95" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="22">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="C20" s="22">
         <v>0.3</v>
@@ -2083,15 +2080,15 @@
         <v>29</v>
       </c>
       <c r="C25" s="18">
-        <f>C24*$B$20</f>
+        <f>C24*$B$20*1.21</f>
         <v>0</v>
       </c>
       <c r="D25" s="18">
-        <f>D24*$B$20</f>
+        <f>D24*$B$20*1.21</f>
         <v>0</v>
       </c>
       <c r="E25" s="18">
-        <f>E24*$B$20</f>
+        <f>E24*$B$20*1.21</f>
         <v>0</v>
       </c>
       <c r="F25" s="3"/>
@@ -2127,15 +2124,15 @@
       </c>
       <c r="C26" s="18">
         <f>C25+$H$12+$H$16</f>
-        <v>22500</v>
+        <v>12500</v>
       </c>
       <c r="D26" s="18">
         <f>D25+$H$12+$H$16</f>
-        <v>22500</v>
+        <v>12500</v>
       </c>
       <c r="E26" s="18">
         <f>E25+$H$12+$H$16</f>
-        <v>22500</v>
+        <v>12500</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -2170,15 +2167,15 @@
       </c>
       <c r="C27" s="18">
         <f>C24-C26</f>
-        <v>-22500</v>
+        <v>-12500</v>
       </c>
       <c r="D27" s="18">
         <f t="shared" ref="D27:E27" si="0">D24-D26</f>
-        <v>-22500</v>
+        <v>-12500</v>
       </c>
       <c r="E27" s="18">
         <f t="shared" si="0"/>
-        <v>-22500</v>
+        <v>-12500</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -2256,15 +2253,15 @@
       </c>
       <c r="C29" s="25">
         <f>(C24-C26)*$C$20</f>
-        <v>-6750</v>
+        <v>-3750</v>
       </c>
       <c r="D29" s="25">
         <f>(D24-D26)*$C$20</f>
-        <v>-6750</v>
+        <v>-3750</v>
       </c>
       <c r="E29" s="25">
         <f>(E24-E26)*$C$20</f>
-        <v>-6750</v>
+        <v>-3750</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -2299,15 +2296,15 @@
       </c>
       <c r="C30" s="31">
         <f>$D$20/C26</f>
-        <v>1.1111111111111112</v>
+        <v>2</v>
       </c>
       <c r="D30" s="31">
         <f>$D$20/D26</f>
-        <v>1.1111111111111112</v>
+        <v>2</v>
       </c>
       <c r="E30" s="31">
         <f>$D$20/E26</f>
-        <v>1.1111111111111112</v>
+        <v>2</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>

</xml_diff>

<commit_message>
feat: add legal status 'Indiviso' handling in opportunity views and update related calculations
</commit_message>
<xml_diff>
--- a/assets/Plantilla-Operacion.xlsx
+++ b/assets/Plantilla-Operacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\proyectos-web\inversorhouse-web\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666F9A53-C347-4B02-871B-E5A863DA5AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAF5920-78D4-4D56-B0F4-F7CB23232DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A9FBD9E-D8FD-47FD-9CB6-C19224A81F71}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>DATOS  INMUBLE</t>
   </si>
@@ -255,6 +255,9 @@
   <si>
     <t>Otros gastos</t>
   </si>
+  <si>
+    <t>INVERSIÓN TOTAL</t>
+  </si>
 </sst>
 </file>
 
@@ -263,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +427,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -505,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -671,6 +680,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -694,7 +733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -822,6 +861,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -872,7 +917,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1866566</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1085907</xdr:rowOff>
+      <xdr:rowOff>1082097</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1823,7 +1868,7 @@
       <c r="AC17" s="7"/>
       <c r="AD17" s="7"/>
     </row>
-    <row r="18" spans="1:30" ht="14.4">
+    <row r="18" spans="1:30" ht="15" thickBot="1">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
         <v>28</v>
@@ -1871,7 +1916,9 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="46" t="s">
+        <v>45</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1895,7 +1942,7 @@
       <c r="AC19" s="7"/>
       <c r="AD19" s="7"/>
     </row>
-    <row r="20" spans="1:30" ht="19.95" customHeight="1">
+    <row r="20" spans="1:30" ht="19.95" customHeight="1" thickBot="1">
       <c r="A20" s="2"/>
       <c r="B20" s="22">
         <v>0.03</v>
@@ -1909,7 +1956,10 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="47">
+        <f>H12+H16</f>
+        <v>12500</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>

</xml_diff>